<commit_message>
Running Version. Updated Breakdown times. Including days.
</commit_message>
<xml_diff>
--- a/_templates/Predictive-Maintainance-Board/Audits_EN.xlsx
+++ b/_templates/Predictive-Maintainance-Board/Audits_EN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Predictive-Maintainance-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21792264-2A51-6B4B-84C9-FA2F9E3F62B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E4786B-1CEC-8F4B-BB42-20087A690570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-54140" yWindow="-4840" windowWidth="29220" windowHeight="28240" xr2:uid="{9B8791ED-9B43-B842-A3BF-E1360AD659B4}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D815"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,7 +494,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>43791</v>
+        <v>43792</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>43791</v>
+        <v>43792</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>43791</v>
+        <v>43795</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>43791</v>
+        <v>43796</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>43793</v>
+        <v>43797</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>43793</v>
+        <v>43797</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -578,7 +578,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>43793</v>
+        <v>43798</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>43795</v>
+        <v>43798</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>43795</v>
+        <v>43798</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>19</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>43795</v>
+        <v>43801</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>43797</v>
+        <v>43801</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>43802</v>
+        <v>43801</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>8</v>

</xml_diff>